<commit_message>
32 Group related Scenarios
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/4061-CREATECLIENT-SUBMITNEWLOAN-CLOSECLIENT.xlsx
+++ b/Mifos Automation Excels/Client/4061-CREATECLIENT-SUBMITNEWLOAN-CLOSECLIENT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="495" windowWidth="15015" windowHeight="7620" activeTab="2"/>
+    <workbookView xWindow="180" yWindow="495" windowWidth="15015" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="9" r:id="rId1"/>
@@ -120,10 +120,10 @@
     <t>submit</t>
   </si>
   <si>
-    <t>389-RBI-EI-DB-DL-REC-NON-RNI-CTPD-SAR-MD-TR-1-B-EarlyRePayment</t>
-  </si>
-  <si>
     <t>verify1</t>
+  </si>
+  <si>
+    <t>3500-RBI-EI-DB-DL-REC-NON-RNI-CTPD-DL-MD-TR-1-ONTIME-DISBURSE-FEE-%APR-AMT-Reg-PERIODIC</t>
   </si>
 </sst>
 </file>
@@ -188,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -216,7 +216,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,7 +607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -630,8 +629,8 @@
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>34</v>
+      <c r="B2" s="7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -699,7 +698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -751,7 +750,7 @@
     </row>
     <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>26</v>

</xml_diff>